<commit_message>
Updated headspace prep file
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Raw_GHG/2021/Raw/Headspace Preparation Conditions Summer 2021.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Raw_GHG/2021/Raw/Headspace Preparation Conditions Summer 2021.xlsx
@@ -366,7 +366,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -501,60 +501,164 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1">
+        <v>44341</v>
+      </c>
+      <c r="B14">
+        <v>20.9</v>
+      </c>
+      <c r="C14">
+        <v>30.18</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>44348</v>
+      </c>
+      <c r="B15">
+        <v>20.7</v>
+      </c>
+      <c r="C15">
+        <v>30.242999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>44361</v>
+      </c>
+      <c r="B16">
+        <v>20.7</v>
+      </c>
+      <c r="C16">
+        <v>29.858000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>44364</v>
+      </c>
+      <c r="B17">
+        <v>20.6</v>
+      </c>
+      <c r="C17">
+        <v>30.053999999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>44370</v>
+      </c>
+      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>30.184000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>44376</v>
+      </c>
+      <c r="B19">
+        <v>23.2</v>
+      </c>
+      <c r="C19">
+        <v>30.222000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="1">
+        <v>44386</v>
+      </c>
+      <c r="B20">
+        <v>22.5</v>
+      </c>
+      <c r="C20">
+        <v>29.928999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="1">
+        <v>44390</v>
+      </c>
+      <c r="B21">
+        <v>23.8</v>
+      </c>
+      <c r="C21">
+        <v>30.183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>44399</v>
+      </c>
+      <c r="B22">
+        <v>22.3</v>
+      </c>
+      <c r="C22">
+        <v>30.111000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>44404</v>
+      </c>
+      <c r="B23">
+        <v>21.9</v>
+      </c>
+      <c r="C23">
+        <v>29.977</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B24">
+        <v>22.1</v>
+      </c>
+      <c r="C24">
+        <v>30.03</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>44418</v>
+      </c>
+      <c r="B25">
+        <v>22.2</v>
+      </c>
+      <c r="C25">
+        <v>30.135999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="1">
+        <v>44425</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>30.1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
GHGs through 8 Dec 2021; corrected megasheet.
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Raw_GHG/2021/Raw/Headspace Preparation Conditions Summer 2021.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Raw_GHG/2021/Raw/Headspace Preparation Conditions Summer 2021.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\StreamTeam Analytical Lab\Projects\Carey Misc\2021 season misc analyses\GC 2021\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoun\Desktop\Reservoirs\Data\DataNotYetUploadedToEDI\Raw_GHG\2021\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EDD0C4-D773-4BFC-8B65-CB0EFD62F1B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="17250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="17256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -68,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -76,13 +77,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,24 +384,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43:C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -390,7 +412,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -401,7 +423,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44236</v>
       </c>
@@ -412,7 +434,7 @@
         <v>30.178000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44256</v>
       </c>
@@ -423,7 +445,7 @@
         <v>29.788</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44264</v>
       </c>
@@ -434,7 +456,7 @@
         <v>30.521999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44278</v>
       </c>
@@ -445,7 +467,7 @@
         <v>30.158000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44292</v>
       </c>
@@ -456,7 +478,7 @@
         <v>30.048999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44305</v>
       </c>
@@ -467,7 +489,7 @@
         <v>29.866</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44320</v>
       </c>
@@ -478,7 +500,7 @@
         <v>29.806000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44323</v>
       </c>
@@ -489,7 +511,7 @@
         <v>29.908000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44334</v>
       </c>
@@ -500,7 +522,7 @@
         <v>30.363</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44341</v>
       </c>
@@ -511,7 +533,7 @@
         <v>30.18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44348</v>
       </c>
@@ -522,7 +544,7 @@
         <v>30.242999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44361</v>
       </c>
@@ -533,7 +555,7 @@
         <v>29.858000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44364</v>
       </c>
@@ -544,7 +566,7 @@
         <v>30.053999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44370</v>
       </c>
@@ -555,7 +577,7 @@
         <v>30.184000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44376</v>
       </c>
@@ -566,7 +588,7 @@
         <v>30.222000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44386</v>
       </c>
@@ -577,7 +599,7 @@
         <v>29.928999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44390</v>
       </c>
@@ -588,7 +610,7 @@
         <v>30.183</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44399</v>
       </c>
@@ -599,7 +621,7 @@
         <v>30.111000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44404</v>
       </c>
@@ -610,7 +632,7 @@
         <v>29.977</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44411</v>
       </c>
@@ -621,7 +643,7 @@
         <v>30.03</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44418</v>
       </c>
@@ -632,7 +654,7 @@
         <v>30.135999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44425</v>
       </c>
@@ -643,7 +665,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44432</v>
       </c>
@@ -654,7 +676,7 @@
         <v>30.11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44440</v>
       </c>
@@ -665,7 +687,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44446</v>
       </c>
@@ -676,7 +698,7 @@
         <v>30.055</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44454</v>
       </c>
@@ -687,7 +709,7 @@
         <v>29.97</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44461</v>
       </c>
@@ -698,7 +720,7 @@
         <v>29.856999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>44467</v>
       </c>
@@ -709,7 +731,7 @@
         <v>29.98</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>44474</v>
       </c>
@@ -720,7 +742,7 @@
         <v>30.106999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>44481</v>
       </c>
@@ -731,7 +753,7 @@
         <v>30.073</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>44482</v>
       </c>
@@ -742,28 +764,96 @@
         <v>30.062000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>44488</v>
+      </c>
+      <c r="B36">
+        <v>21</v>
+      </c>
+      <c r="C36">
+        <v>30.234000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>44495</v>
+      </c>
+      <c r="B37">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C37">
+        <v>29.742000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>44496</v>
+      </c>
+      <c r="B38">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="C38">
+        <v>29.939</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>44504</v>
+      </c>
+      <c r="B39">
+        <v>20.9</v>
+      </c>
+      <c r="C39">
+        <v>30.305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>44509</v>
+      </c>
+      <c r="B40">
+        <v>20.8</v>
+      </c>
+      <c r="C40">
+        <v>30.274999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>44510</v>
+      </c>
+      <c r="B41">
+        <v>20.2</v>
+      </c>
+      <c r="C41">
+        <v>30.169</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1">
+        <v>44523</v>
+      </c>
+      <c r="B42">
+        <v>20.8</v>
+      </c>
+      <c r="C42">
+        <v>30.228000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="2">
+        <v>44537</v>
+      </c>
+      <c r="B43" s="3">
+        <v>20.3</v>
+      </c>
+      <c r="C43" s="3">
+        <v>30.210999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final data for EDI dissolved GHG; published in staging.
</commit_message>
<xml_diff>
--- a/Data/DataNotYetUploadedToEDI/Raw_GHG/2021/Raw/Headspace Preparation Conditions Summer 2021.xlsx
+++ b/Data/DataNotYetUploadedToEDI/Raw_GHG/2021/Raw/Headspace Preparation Conditions Summer 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20382"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahoun\Desktop\Reservoirs\Data\DataNotYetUploadedToEDI\Raw_GHG\2021\Raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\StreamTeam Analytical Lab\Projects\Carey Misc\2021 season misc analyses\GC 2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EDD0C4-D773-4BFC-8B65-CB0EFD62F1B0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DA6475-5723-45B2-AF91-4FFEEAB7DE98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="17256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17820" windowHeight="17250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -77,34 +77,13 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFCCCCCC"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFCCCCCC"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFCCCCCC"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -387,21 +366,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -412,7 +391,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -423,7 +402,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>44236</v>
       </c>
@@ -434,7 +413,7 @@
         <v>30.178000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>44256</v>
       </c>
@@ -445,7 +424,7 @@
         <v>29.788</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>44264</v>
       </c>
@@ -456,7 +435,7 @@
         <v>30.521999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>44278</v>
       </c>
@@ -467,7 +446,7 @@
         <v>30.158000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>44292</v>
       </c>
@@ -478,7 +457,7 @@
         <v>30.048999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>44305</v>
       </c>
@@ -489,7 +468,7 @@
         <v>29.866</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>44320</v>
       </c>
@@ -500,7 +479,7 @@
         <v>29.806000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>44323</v>
       </c>
@@ -511,7 +490,7 @@
         <v>29.908000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>44334</v>
       </c>
@@ -522,7 +501,7 @@
         <v>30.363</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>44341</v>
       </c>
@@ -533,7 +512,7 @@
         <v>30.18</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>44348</v>
       </c>
@@ -544,9 +523,9 @@
         <v>30.242999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
-        <v>44361</v>
+        <v>44360</v>
       </c>
       <c r="B16">
         <v>20.7</v>
@@ -555,7 +534,7 @@
         <v>29.858000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>44364</v>
       </c>
@@ -566,7 +545,7 @@
         <v>30.053999999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>44370</v>
       </c>
@@ -577,7 +556,7 @@
         <v>30.184000000000001</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>44376</v>
       </c>
@@ -588,7 +567,7 @@
         <v>30.222000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>44386</v>
       </c>
@@ -599,7 +578,7 @@
         <v>29.928999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>44390</v>
       </c>
@@ -610,7 +589,7 @@
         <v>30.183</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>44399</v>
       </c>
@@ -621,7 +600,7 @@
         <v>30.111000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>44404</v>
       </c>
@@ -632,7 +611,7 @@
         <v>29.977</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>44411</v>
       </c>
@@ -643,7 +622,7 @@
         <v>30.03</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>44418</v>
       </c>
@@ -654,7 +633,7 @@
         <v>30.135999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>44425</v>
       </c>
@@ -665,7 +644,7 @@
         <v>30.1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>44432</v>
       </c>
@@ -676,7 +655,7 @@
         <v>30.11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>44440</v>
       </c>
@@ -687,7 +666,7 @@
         <v>29.6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>44446</v>
       </c>
@@ -698,7 +677,7 @@
         <v>30.055</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>44454</v>
       </c>
@@ -709,7 +688,7 @@
         <v>29.97</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>44461</v>
       </c>
@@ -720,7 +699,7 @@
         <v>29.856999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>44467</v>
       </c>
@@ -731,7 +710,7 @@
         <v>29.98</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>44474</v>
       </c>
@@ -742,7 +721,7 @@
         <v>30.106999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>44481</v>
       </c>
@@ -753,7 +732,7 @@
         <v>30.073</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>44482</v>
       </c>
@@ -764,7 +743,7 @@
         <v>30.062000000000001</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>44488</v>
       </c>
@@ -775,7 +754,7 @@
         <v>30.234000000000002</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>44495</v>
       </c>
@@ -786,7 +765,7 @@
         <v>29.742000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>44496</v>
       </c>
@@ -797,7 +776,7 @@
         <v>29.939</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>44504</v>
       </c>
@@ -808,7 +787,7 @@
         <v>30.305</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>44509</v>
       </c>
@@ -819,7 +798,7 @@
         <v>30.274999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>44510</v>
       </c>
@@ -830,7 +809,7 @@
         <v>30.169</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>44523</v>
       </c>
@@ -841,19 +820,18 @@
         <v>30.228000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="2">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43" s="1">
         <v>44537</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43">
         <v>20.3</v>
       </c>
-      <c r="C43" s="3">
+      <c r="C43">
         <v>30.210999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>